<commit_message>
Forgot Password - Verify OTP and password reset show success message.
</commit_message>
<xml_diff>
--- a/data/ForgotPassword.xlsx
+++ b/data/ForgotPassword.xlsx
@@ -62,7 +62,7 @@
     <t>testgmail.comjhljkhsfjhj</t>
   </si>
   <si>
-    <t>testtttt</t>
+    <t>testttt</t>
   </si>
   <si>
     <t>test12@t.com</t>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1093,7 +1093,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="test12@t.com" tooltip="mailto:test12@t.com"/>
-    <hyperlink ref="G2" r:id="rId2" display="TEST@123"/>
+    <hyperlink ref="G2" r:id="rId2" display="TEST@123" tooltip="mailto:TEST@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>